<commit_message>
Few changes in PS values of menu v1_2_0
Summary of the changes:
- L1_ETMHF70/L1_ETMHF70_HTT60er seeds were prescaled to 0 (in both default and PS table for rate studies)
- L1_SingleLooseIsoEG26er1p5 was switched ON in default PS table (as it was at end of 2018)
- L1_DoubleMu0er1p5_SQ_dR_Max1p4 prescaled to 50 (instead of 2) in default PS table
</commit_message>
<xml_diff>
--- a/development/L1Menu_Collisions2022_v1_2_0/PrescaleTable/L1Menu_Collisions2022_v1_2_0-DedicatedRateStudyRun3.xlsx
+++ b/development/L1Menu_Collisions2022_v1_2_0/PrescaleTable/L1Menu_Collisions2022_v1_2_0-DedicatedRateStudyRun3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caterinaaruta/Desktop/L1Menus/L1Menu_Collisions2022_v1_2_0/PrescaleTable/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{396D7D97-943C-7E4F-810D-27A29AEF0B6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FB3BBA7-0EC9-FA43-A69A-68BDBF5B1387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1611,7 +1611,7 @@
   <dimension ref="A1:R397"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A321" workbookViewId="0">
-      <selection activeCell="B338" sqref="B338"/>
+      <selection activeCell="F336" sqref="F336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20221,50 +20221,50 @@
       <c r="C333">
         <v>0</v>
       </c>
-      <c r="D333" s="2">
-        <v>1</v>
+      <c r="D333">
+        <v>0</v>
       </c>
       <c r="E333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q333">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R333">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="334" spans="1:18" x14ac:dyDescent="0.2">
@@ -20725,50 +20725,50 @@
       <c r="C342">
         <v>0</v>
       </c>
-      <c r="D342" s="2">
-        <v>1</v>
+      <c r="D342">
+        <v>0</v>
       </c>
       <c r="E342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q342">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R342">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="343" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>